<commit_message>
Change input file paths to work on any PC
</commit_message>
<xml_diff>
--- a/examples/data/input/input.xlsx
+++ b/examples/data/input/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u6406\PycharmProjects\uspekpy\examples\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\PycharmProjects\uspekpy\examples\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -119,10 +119,10 @@
     <t>Case2</t>
   </si>
   <si>
-    <t>C:\Users\u6406\PycharmProjects\uspekpy\examples\data\input\h_k_h_amb_10.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\u6406\PycharmProjects\uspekpy\examples\data\input\mu_tr_rho.csv</t>
+    <t>data\input\mu_tr_rho.csv</t>
+  </si>
+  <si>
+    <t>data\input\h_k_h_amb_10.csv</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,10 +652,10 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,10 +663,10 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>